<commit_message>
Week 24 changes: changes in week 22 folders
</commit_message>
<xml_diff>
--- a/documents/Interview/Interview_Questions.xlsx
+++ b/documents/Interview/Interview_Questions.xlsx
@@ -8,29 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayb\eclipse-workspace\SDET_Training\documents\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1085E3E-753D-4780-8E49-66CEE2B8A160}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415AE5A6-7B12-48A3-BE02-B9C75751DD6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9921EFF5-5251-4471-B206-9AE7DB107384}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="16" r:id="rId1"/>
     <sheet name="FreshWorks" sheetId="1" r:id="rId2"/>
-    <sheet name="ChargeBee" sheetId="5" r:id="rId3"/>
-    <sheet name="Dunzo" sheetId="10" r:id="rId4"/>
-    <sheet name="FreeCharge" sheetId="8" r:id="rId5"/>
-    <sheet name="Swiggy" sheetId="15" r:id="rId6"/>
-    <sheet name="CaratLane" sheetId="13" r:id="rId7"/>
-    <sheet name="Toyota" sheetId="14" r:id="rId8"/>
-    <sheet name="Aut Anywhere" sheetId="17" r:id="rId9"/>
-    <sheet name="Zoho" sheetId="7" r:id="rId10"/>
-    <sheet name="Logitech" sheetId="6" r:id="rId11"/>
-    <sheet name="Global Logic" sheetId="9" r:id="rId12"/>
-    <sheet name="CITI" sheetId="2" r:id="rId13"/>
-    <sheet name="Global English" sheetId="3" r:id="rId14"/>
-    <sheet name="Wipro" sheetId="4" r:id="rId15"/>
-    <sheet name="Logica Infotech" sheetId="12" r:id="rId16"/>
-    <sheet name="DeepIntent" sheetId="11" r:id="rId17"/>
-    <sheet name="Gainsight" sheetId="18" r:id="rId18"/>
+    <sheet name="ThoughtWorks" sheetId="19" r:id="rId3"/>
+    <sheet name="ChargeBee" sheetId="5" r:id="rId4"/>
+    <sheet name="Dunzo" sheetId="10" r:id="rId5"/>
+    <sheet name="FreeCharge" sheetId="8" r:id="rId6"/>
+    <sheet name="Swiggy" sheetId="15" r:id="rId7"/>
+    <sheet name="CaratLane" sheetId="13" r:id="rId8"/>
+    <sheet name="Toyota" sheetId="14" r:id="rId9"/>
+    <sheet name="Aut Anywhere" sheetId="17" r:id="rId10"/>
+    <sheet name="Zoho" sheetId="7" r:id="rId11"/>
+    <sheet name="Logitech" sheetId="6" r:id="rId12"/>
+    <sheet name="Global Logic" sheetId="9" r:id="rId13"/>
+    <sheet name="CITI" sheetId="2" r:id="rId14"/>
+    <sheet name="Global English" sheetId="3" r:id="rId15"/>
+    <sheet name="Wipro" sheetId="4" r:id="rId16"/>
+    <sheet name="Logica Infotech" sheetId="12" r:id="rId17"/>
+    <sheet name="DeepIntent" sheetId="11" r:id="rId18"/>
+    <sheet name="Gainsight" sheetId="18" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="998">
   <si>
     <t>1) Why is the main method static in Java?</t>
   </si>
@@ -2445,6 +2446,617 @@
   </si>
   <si>
     <t>X-path version 2.0</t>
+  </si>
+  <si>
+    <t>Test case enumeration for Coupon-code Redeem text box</t>
+  </si>
+  <si>
+    <t>Test strategy for an application architecture</t>
+  </si>
+  <si>
+    <t>Explain your current project</t>
+  </si>
+  <si>
+    <t>Logical:</t>
+  </si>
+  <si>
+    <t>1. There are 25 horses among which you need to find out the fastest 3 horses. You can conduct race among at most 5 to find out their relative speed. At no point you can find out the actual speed of the horse in a race. Find out how many races are required to get the top 3 horses.</t>
+  </si>
+  <si>
+    <t>2. There is a train service between chennai to coimbatore. Each hour one train will be starting from Chennai to Coimbatore for 24/7. The same service from Coimbatore to Chennai. Travel time between chennai &amp; coimbatore is 8 Hrs. You are starting at 6 AM from chennai. How many trains will you seeing in opposite before you reach Coimbatore.</t>
+  </si>
+  <si>
+    <t>1. Find the maximum sub-array which contains the maximum product.</t>
+  </si>
+  <si>
+    <t>input = {12,23,34,-23,0,34}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. We have an array of hashes, so how to check my array of hashes contains a hash with a given key-value pair? </t>
+  </si>
+  <si>
+    <t>[{"question"=&gt;"0a2a3452", "answer"=&gt;"bull"}, {"question"=&gt;"58deacf9", "answer"=&gt;"bullafolo"}, {"question"=&gt;"32c53e5f", "answer"=&gt;"curosit"}, {"question"=&gt;"b5546bcf", "answer"=&gt;""}, {"question"=&gt;"0f0b314", "answer"=&gt;""}]</t>
+  </si>
+  <si>
+    <t>Check if "question"=&gt;"b5546bcf" (along with value) is present in the given array of hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selenium: </t>
+  </si>
+  <si>
+    <t>1. Exception that you have faced?</t>
+  </si>
+  <si>
+    <t>2. What is StaleElementReferenceException?</t>
+  </si>
+  <si>
+    <t>3. When will you get StaleElementReferenceException?</t>
+  </si>
+  <si>
+    <t>4. Is that possible to get StaleElementReferenceException while interacting an element inside the frame?</t>
+  </si>
+  <si>
+    <t>5. How would you add the value in map using JSON parser?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. There is a Web Chat appication which works with default microphone. Write a selenium code for the below operations in webchat application. </t>
+  </si>
+  <si>
+    <t>Assume two users. User1 &amp; User2.</t>
+  </si>
+  <si>
+    <t>a) Verify User1 sends the message to User2</t>
+  </si>
+  <si>
+    <t>b) Verify the message received by User2</t>
+  </si>
+  <si>
+    <t>c) Verify User2 sends the acknowledgement through chat to User1</t>
+  </si>
+  <si>
+    <t>d) make sure that user2 receives that message</t>
+  </si>
+  <si>
+    <t>7. Which framework you have worked on? Difference between BDD and Hybrid?</t>
+  </si>
+  <si>
+    <t>Note: Clean code with TestNG annotations.</t>
+  </si>
+  <si>
+    <t>1. HTTP Methods?</t>
+  </si>
+  <si>
+    <t>2. Diff b/e PUT,POST and PATCH?</t>
+  </si>
+  <si>
+    <t>3. What would you validate in API? Request, Response, etc,.</t>
+  </si>
+  <si>
+    <t>4. Diff b/w Authorization &amp; Authorization</t>
+  </si>
+  <si>
+    <t>Types of frame work used</t>
+  </si>
+  <si>
+    <t>2. Types of constructors</t>
+  </si>
+  <si>
+    <t>3. Method Overloading</t>
+  </si>
+  <si>
+    <t>4. Method Overriding</t>
+  </si>
+  <si>
+    <t>5. if two interfaces have same methods, which method will be implemented in the implementing class</t>
+  </si>
+  <si>
+    <t>6. if only the order of the arguments change in two methods, is that overloading</t>
+  </si>
+  <si>
+    <t>7. 3 ways/keywords to prevent a method from overloading</t>
+  </si>
+  <si>
+    <t>8. What is interface</t>
+  </si>
+  <si>
+    <t>9. In java can a class inherit from more than one class</t>
+  </si>
+  <si>
+    <t>10. Do we have any limit for multi level inheritance in Java</t>
+  </si>
+  <si>
+    <t>11. what is the use of static keyword? why we need to access methods/variables without object in java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. How to access static member of a class using object </t>
+  </si>
+  <si>
+    <t>*by using a public method with object as argument</t>
+  </si>
+  <si>
+    <t>class A</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>static int v;</t>
+  </si>
+  <si>
+    <t>public int getv(A a)</t>
+  </si>
+  <si>
+    <t>return a.v;</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>A obj =new A();</t>
+  </si>
+  <si>
+    <t>getv(obj);</t>
+  </si>
+  <si>
+    <t>13.what are the collections u have used</t>
+  </si>
+  <si>
+    <t>14. when to use arraylist and when to use linked list</t>
+  </si>
+  <si>
+    <t>15. Time Complexity for inserting in LinkedList</t>
+  </si>
+  <si>
+    <t>16. Sets used in framework</t>
+  </si>
+  <si>
+    <t>17. Code to remove duplicates from a String,</t>
+  </si>
+  <si>
+    <t>use the same method to remove duplicates from each word of a string(seprated by space)</t>
+  </si>
+  <si>
+    <t>18.When to Use Map</t>
+  </si>
+  <si>
+    <t>19. Intial capacity of ArrayList</t>
+  </si>
+  <si>
+    <t>20.What is the need for collections, compared to array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21. can we store elements of different data types in collection </t>
+  </si>
+  <si>
+    <t>1. How Selenium code , iteract with drivers</t>
+  </si>
+  <si>
+    <t>2. how drivers interact with browsers</t>
+  </si>
+  <si>
+    <t>3. Who is provinding drivers for each browsers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Code for(with out locators) for any login </t>
+  </si>
+  <si>
+    <t>5. why we maximize window</t>
+  </si>
+  <si>
+    <t>6. Can we run headon in containers (running from jenkins)</t>
+  </si>
+  <si>
+    <t>7. how implicit wait wrks</t>
+  </si>
+  <si>
+    <t>8. how explicit wait works</t>
+  </si>
+  <si>
+    <t>9. how to change the pooling time in webdriver wait</t>
+  </si>
+  <si>
+    <t>10.how to handle a alert , which can appear after a time( the time to appear changes )</t>
+  </si>
+  <si>
+    <t>11.Exceptions handled</t>
+  </si>
+  <si>
+    <t>12.What is stale element exception</t>
+  </si>
+  <si>
+    <t>13.How to handle stale element exception</t>
+  </si>
+  <si>
+    <t>14. features of testNG</t>
+  </si>
+  <si>
+    <t>15. How to run a test case , multiple iteration</t>
+  </si>
+  <si>
+    <t>1. with same data</t>
+  </si>
+  <si>
+    <t>2. with different data</t>
+  </si>
+  <si>
+    <t>16. How to run testcases in less time(How to do parallel execution)</t>
+  </si>
+  <si>
+    <t>17.How to rerun failed cases using testNG</t>
+  </si>
+  <si>
+    <t>18.How to make one method not to run if another particular method fails</t>
+  </si>
+  <si>
+    <t>19. Dependens on , used in your framwork</t>
+  </si>
+  <si>
+    <t>20.How to make one set of methods not to run if another particular set of method fails</t>
+  </si>
+  <si>
+    <t>21.If a test is run multiple times uisng invocation count, if one iteration failed ll the next iterations be continued?</t>
+  </si>
+  <si>
+    <t>22.What is headless browser</t>
+  </si>
+  <si>
+    <t>1. Exceptions faced</t>
+  </si>
+  <si>
+    <t>2. What are the possible request in a mail box application</t>
+  </si>
+  <si>
+    <t>3. What is the difference between getting  single mail and list of mail</t>
+  </si>
+  <si>
+    <t>4. How can we get mails after the max limit in configured in a response</t>
+  </si>
+  <si>
+    <t>5. why query parameter is needed</t>
+  </si>
+  <si>
+    <t>6. How to attach files in request-what is th content type of request and response</t>
+  </si>
+  <si>
+    <t>7. if a email ID of invalid format is passed in request what error code will get? (2 possible error codes)</t>
+  </si>
+  <si>
+    <t>8. In the above case if it is 500 error code, how will you debug</t>
+  </si>
+  <si>
+    <t>9. when will we get 403 error code</t>
+  </si>
+  <si>
+    <t>10. difference between 401 and 403</t>
+  </si>
+  <si>
+    <t>11. in the above mail api when we try to get a mail which is not available, what will be the code and message?</t>
+  </si>
+  <si>
+    <t>CI/CD</t>
+  </si>
+  <si>
+    <t>1. Where/how CI/CD is used?</t>
+  </si>
+  <si>
+    <t>2. How trigger jobs periodically?</t>
+  </si>
+  <si>
+    <t>3.How to achieve paralle execution in master slave archietecture using TestNG</t>
+  </si>
+  <si>
+    <t>4. Can same testng XML for used in parallel test execution across differnt slaves? how?</t>
+  </si>
+  <si>
+    <t>5.Do u write the Groovy pipeline code</t>
+  </si>
+  <si>
+    <t>1. Tell About your self</t>
+  </si>
+  <si>
+    <t>2. Role in Test Cycle</t>
+  </si>
+  <si>
+    <t>3. What are the follow up setps when customer reports a bug in production</t>
+  </si>
+  <si>
+    <t>4. What will you do if the bug is not reproducible in test environment</t>
+  </si>
+  <si>
+    <t>5. Who writes test case in your team</t>
+  </si>
+  <si>
+    <t>6. How you/team test not automated testcases? how Automation coverage is maintained/tracked?</t>
+  </si>
+  <si>
+    <t>7. Who will select /prioratize the test cases that needs to be automated?</t>
+  </si>
+  <si>
+    <t>8. in Grooming will you be providing your suggesstions ?</t>
+  </si>
+  <si>
+    <t>9. Test cases for Search API</t>
+  </si>
+  <si>
+    <t>10. test cases for ticket booking app and google calender integration</t>
+  </si>
+  <si>
+    <t>11.if add to cart button in flipkart is not working, how will you debug</t>
+  </si>
+  <si>
+    <t>12. In Gmail attachment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> any number of files can be attached, but the size limit for single file is 10 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and limit for cumulative size is 50 Mb</t>
+  </si>
+  <si>
+    <t>write test scenarios</t>
+  </si>
+  <si>
+    <t>13. Defect Cycle</t>
+  </si>
+  <si>
+    <t>14. Who will make decision to defer a defect</t>
+  </si>
+  <si>
+    <t>15. Severity/Priority</t>
+  </si>
+  <si>
+    <t>16. Who decides severity /priority</t>
+  </si>
+  <si>
+    <t>1)Testcase enumeration</t>
+  </si>
+  <si>
+    <t>Scenario: App -&gt; PArking System</t>
+  </si>
+  <si>
+    <t>UI:</t>
+  </si>
+  <si>
+    <t>1. Show the available slots --&gt; Assign the slots Randomly</t>
+  </si>
+  <si>
+    <t>2. Once the vechicle swipes --&gt; show the availability if the slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service: </t>
+  </si>
+  <si>
+    <t>POST --&gt; Submitting --&gt; Slot Num</t>
+  </si>
+  <si>
+    <t>GET --&gt; Show the available no.of slots</t>
+  </si>
+  <si>
+    <t>comeup with test plan,manual cases and automation cases(expected to follow test pyramind)</t>
+  </si>
+  <si>
+    <t>2)different testing techniques used for testing a textbox - allows lowercase/uppercase of min 6 chars and max 12 chars</t>
+  </si>
+  <si>
+    <t>3) What is test strategy &amp; test plan, testing life cycle</t>
+  </si>
+  <si>
+    <t>4)what is test pyramid - explain</t>
+  </si>
+  <si>
+    <t>5)Agile - full process</t>
+  </si>
+  <si>
+    <t>Design &amp; implement simple UI framework(asked to code), API framework- only explanation</t>
+  </si>
+  <si>
+    <t>Program : Input - Thoughtworks, replace 't' with uppercase Testcase w/o inbulit methods</t>
+  </si>
+  <si>
+    <t>Program : Input - Thoughtworks, remove 't' w/o inbulit methods</t>
+  </si>
+  <si>
+    <t>why main method is static?</t>
+  </si>
+  <si>
+    <t>what is the use of static method?</t>
+  </si>
+  <si>
+    <t>why do we create objects for classes?</t>
+  </si>
+  <si>
+    <t>Real time project methods where static method is used</t>
+  </si>
+  <si>
+    <t>Early binding and dynamic binding</t>
+  </si>
+  <si>
+    <t>Constructor chaining</t>
+  </si>
+  <si>
+    <t>Why String is immutable?</t>
+  </si>
+  <si>
+    <t>which of the above methods will be executed?</t>
+  </si>
+  <si>
+    <t>why child class object cannot be used for accessing parent class methods?</t>
+  </si>
+  <si>
+    <t>what is the difference between Interface and Abstract class?</t>
+  </si>
+  <si>
+    <t>when we use Interface and when Abstract class?</t>
+  </si>
+  <si>
+    <t>why are we using Interface to create object and access the implementing the class methods?</t>
+  </si>
+  <si>
+    <t>example: WebDriver driver = new ChromeDriver(); instead of ChromeDriver driver = new ChromeDriver();</t>
+  </si>
+  <si>
+    <t>When do we use ArrayList and LinkedList?</t>
+  </si>
+  <si>
+    <t>O notations for the respective methods</t>
+  </si>
+  <si>
+    <t>HashSet implementations</t>
+  </si>
+  <si>
+    <t>can we store duplicates in Set?</t>
+  </si>
+  <si>
+    <t>how to overcome the challenge of storing duplicate as object in Set?</t>
+  </si>
+  <si>
+    <t>Validate paranthesis</t>
+  </si>
+  <si>
+    <t>Selenium architecture</t>
+  </si>
+  <si>
+    <t>How to overcome Stale Element exception?</t>
+  </si>
+  <si>
+    <t>How JavaScript executor works?</t>
+  </si>
+  <si>
+    <t>Disadvantage of JavaScript executor</t>
+  </si>
+  <si>
+    <t>Assuming a email api -  write possible API methods</t>
+  </si>
+  <si>
+    <t>If need to fetch all the emails what method call should I use?</t>
+  </si>
+  <si>
+    <t>If I give a search keyword that is not present, what error code will I get?</t>
+  </si>
+  <si>
+    <t>Program question</t>
+  </si>
+  <si>
+    <t>Add contact from UI</t>
+  </si>
+  <si>
+    <t>Add contact via file upload</t>
+  </si>
+  <si>
+    <t>Edit contact</t>
+  </si>
+  <si>
+    <t>Delete contact</t>
+  </si>
+  <si>
+    <t>Delete after bulk select</t>
+  </si>
+  <si>
+    <t>Possible actions on Add contact--&gt; CRUD operations</t>
+  </si>
+  <si>
+    <t>How to test those?</t>
+  </si>
+  <si>
+    <t>2. Steps for Defect logged by customer in prod</t>
+  </si>
+  <si>
+    <t>3. How defects by customer and QA team is categorized/differentiated</t>
+  </si>
+  <si>
+    <t>4. Defect life cycle</t>
+  </si>
+  <si>
+    <t>5. Selenium script for enter email and click button</t>
+  </si>
+  <si>
+    <t>6. waits (explicit wait condition to wait till element is present)</t>
+  </si>
+  <si>
+    <t>7. How to pass test Data to Automation Scripts</t>
+  </si>
+  <si>
+    <t>8.What type of frame work used for UI testing</t>
+  </si>
+  <si>
+    <t>9. Explain your current application and test approach</t>
+  </si>
+  <si>
+    <t>10. Challenges faced during test and automation of your application</t>
+  </si>
+  <si>
+    <t>11. Word Break problem</t>
+  </si>
+  <si>
+    <t>1. Explain Test Planning , approach and Scenarios(high level) for a contacts application</t>
+  </si>
+  <si>
+    <t>1. Explain about yourself and roles played so far</t>
+  </si>
+  <si>
+    <t>2. Explain your career growth/transition? and challenges in that.</t>
+  </si>
+  <si>
+    <t>3. Where u see youself in 2 /5 years?</t>
+  </si>
+  <si>
+    <t>4. Have you helped and guided your team?</t>
+  </si>
+  <si>
+    <t>5. When do you came to know about Freshworks?</t>
+  </si>
+  <si>
+    <t>6. Do you know about products of freshworks?</t>
+  </si>
+  <si>
+    <t>7. Any Questions about freshworks</t>
+  </si>
+  <si>
+    <t>What is JRE, JVM and JDK? When you will use these?</t>
+  </si>
+  <si>
+    <t>What is the diff between encryption and hashing? Where its used in your day to day activity (except Java &amp; Selenium)?</t>
+  </si>
+  <si>
+    <t>What is Dockers &amp; containers?</t>
+  </si>
+  <si>
+    <t>Why main method is static?</t>
+  </si>
+  <si>
+    <t>What is immutable and why string is immutable?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How will you achieve the parallel execution? </t>
+  </si>
+  <si>
+    <t>Thread rising</t>
+  </si>
+  <si>
+    <t>Find the intersection for k number of arrays.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Debugging Qn:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Navigation from one page to another page slow for a particular application. How will you debug this?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2985,6 +3597,53 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F27406-B35D-4E7F-BF58-232C7DFAD1A3}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="80.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CC4AA9-F201-4CF9-8C84-A706D3A63D28}">
   <dimension ref="A1:A55"/>
   <sheetViews>
@@ -3217,7 +3876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2778574C-63CC-463D-A68D-E4F793A5F3C8}">
   <dimension ref="A1:A56"/>
   <sheetViews>
@@ -3489,7 +4148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B7D59E-A1D8-4245-B8E3-CFBBD78B80F5}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -3592,7 +4251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9D4652-F80D-4003-93B0-0F8769751DA2}">
   <dimension ref="A1:A37"/>
   <sheetViews>
@@ -3793,7 +4452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B063943D-3BF7-4005-9BA4-776A95F07167}">
   <dimension ref="A2:A23"/>
   <sheetViews>
@@ -3914,7 +4573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31098C9C-93FE-485F-9190-A0148D218930}">
   <dimension ref="A1:A64"/>
   <sheetViews>
@@ -4232,7 +4891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C33F1-A1FB-4B2B-8414-A0665D70F3A5}">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -4298,7 +4957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073BA8A9-7826-4D89-BEBA-4976E18552D1}">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -4352,7 +5011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CEDD9D-03AE-426B-A47D-1BC31D89A7C9}">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -4444,679 +5103,1680 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70811466-9302-4B61-86B7-B701B3741742}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:E239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="73.5546875" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" customWidth="1"/>
-    <col min="3" max="3" width="61.88671875" customWidth="1"/>
-    <col min="4" max="4" width="71.5546875" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="D20" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>207</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>209</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>210</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>211</v>
-      </c>
-      <c r="B29" s="1" t="s">
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>212</v>
-      </c>
-      <c r="B30" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B40" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B51" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="B54" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="B56" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="B57" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="D58" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B60" s="2"/>
+      <c r="D60" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="D61" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="D62" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="D63" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="D64" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="D65" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="D66" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="D67" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="D68" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="D70" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>722</v>
+      </c>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="B104" s="4"/>
+    </row>
+    <row r="105" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B106" s="1"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B108" s="4"/>
+    </row>
+    <row r="109" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B113" s="1"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="B115" s="4"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B128" s="1"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B130" s="4"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B139" s="2"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A217" s="1" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" s="1" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B221" s="2"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="1" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="1" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A224" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A225" s="1" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A227" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A228" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A229" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" s="1" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A232" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" s="4" t="s">
+        <v>896</v>
+      </c>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" s="1" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A237" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A238" s="1" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" s="1" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -5126,6 +6786,132 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DD3467-2B99-44E2-94DD-B35AB2451446}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="69.5546875" customWidth="1"/>
+    <col min="2" max="2" width="62.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B3" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B4" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F02FB25-3DFF-41E7-92B5-834D40ACAD7B}">
   <dimension ref="A1:C96"/>
   <sheetViews>
@@ -5814,7 +7600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00A1B05-956D-4043-80BD-1DED8F2F6975}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -6064,7 +7850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB85AB0-402B-4E08-B2B3-647BD366FFAA}">
   <dimension ref="A1:B60"/>
   <sheetViews>
@@ -6421,7 +8207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B18DB3B-9D0D-4526-B1CF-6EF0A840E8A6}">
   <dimension ref="A1:B55"/>
   <sheetViews>
@@ -6764,7 +8550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6EED80-F386-4D8D-8E22-BBDE76B2048C}">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -6900,7 +8686,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>624</v>
       </c>
@@ -6910,7 +8696,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>626</v>
       </c>
@@ -6940,7 +8726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD1F9D0-1F41-4D46-A88C-38D4B372000A}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -7114,51 +8900,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F27406-B35D-4E7F-BF58-232C7DFAD1A3}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="80.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>676</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Few solved solutions added
</commit_message>
<xml_diff>
--- a/documents/Interview/Interview_Questions.xlsx
+++ b/documents/Interview/Interview_Questions.xlsx
@@ -8,34 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayb\eclipse-workspace\SDET_Training\documents\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9EFCBF-2C7C-4C5C-908D-E625244CDB0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275120C2-5867-43FB-A650-B570B967B23C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9921EFF5-5251-4471-B206-9AE7DB107384}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{9921EFF5-5251-4471-B206-9AE7DB107384}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="16" r:id="rId1"/>
     <sheet name="FreshWorks" sheetId="1" r:id="rId2"/>
-    <sheet name="ThoughtWorks" sheetId="19" r:id="rId3"/>
-    <sheet name="ChargeBee" sheetId="5" r:id="rId4"/>
-    <sheet name="Dunzo" sheetId="10" r:id="rId5"/>
-    <sheet name="FreeCharge" sheetId="8" r:id="rId6"/>
-    <sheet name="MakeMyTrip" sheetId="20" r:id="rId7"/>
-    <sheet name="Phonepe" sheetId="21" r:id="rId8"/>
-    <sheet name="Swiggy" sheetId="15" r:id="rId9"/>
-    <sheet name="CaratLane" sheetId="13" r:id="rId10"/>
-    <sheet name="Toyota" sheetId="14" r:id="rId11"/>
-    <sheet name="Aut Anywhere" sheetId="17" r:id="rId12"/>
-    <sheet name="Zoho" sheetId="7" r:id="rId13"/>
-    <sheet name="Logitech" sheetId="6" r:id="rId14"/>
-    <sheet name="Global Logic" sheetId="9" r:id="rId15"/>
-    <sheet name="CITI" sheetId="2" r:id="rId16"/>
-    <sheet name="Global English" sheetId="3" r:id="rId17"/>
-    <sheet name="Wipro" sheetId="4" r:id="rId18"/>
-    <sheet name="Logica Infotech" sheetId="12" r:id="rId19"/>
-    <sheet name="DeepIntent" sheetId="11" r:id="rId20"/>
-    <sheet name="Gainsight" sheetId="18" r:id="rId21"/>
-    <sheet name="Optum" sheetId="22" r:id="rId22"/>
-    <sheet name="Others" sheetId="23" r:id="rId23"/>
+    <sheet name="Ally" sheetId="25" r:id="rId3"/>
+    <sheet name="ThoughtWorks" sheetId="19" r:id="rId4"/>
+    <sheet name="ChargeBee" sheetId="5" r:id="rId5"/>
+    <sheet name="Dunzo" sheetId="10" r:id="rId6"/>
+    <sheet name="FreeCharge" sheetId="8" r:id="rId7"/>
+    <sheet name="MakeMyTrip" sheetId="20" r:id="rId8"/>
+    <sheet name="Phonepe" sheetId="21" r:id="rId9"/>
+    <sheet name="Swiggy" sheetId="15" r:id="rId10"/>
+    <sheet name="CaratLane" sheetId="13" r:id="rId11"/>
+    <sheet name="Toyota" sheetId="14" r:id="rId12"/>
+    <sheet name="Aut Anywhere" sheetId="17" r:id="rId13"/>
+    <sheet name="Zoho" sheetId="7" r:id="rId14"/>
+    <sheet name="Logitech" sheetId="6" r:id="rId15"/>
+    <sheet name="Global Logic" sheetId="9" r:id="rId16"/>
+    <sheet name="CITI" sheetId="2" r:id="rId17"/>
+    <sheet name="Global English" sheetId="3" r:id="rId18"/>
+    <sheet name="Wipro" sheetId="4" r:id="rId19"/>
+    <sheet name="Logica Infotech" sheetId="12" r:id="rId20"/>
+    <sheet name="DeepIntent" sheetId="11" r:id="rId21"/>
+    <sheet name="Gainsight" sheetId="18" r:id="rId22"/>
+    <sheet name="Optum" sheetId="22" r:id="rId23"/>
+    <sheet name="Others" sheetId="23" r:id="rId24"/>
+    <sheet name="RedBus" sheetId="24" r:id="rId25"/>
+    <sheet name="Meesho" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="1313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1497">
   <si>
     <t>1) Why is the main method static in Java?</t>
   </si>
@@ -4007,12 +4010,569 @@
   <si>
     <t>Feature planning to deployment</t>
   </si>
+  <si>
+    <t>Find Whether the given String is Palindrome or Not</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>left = 0, right = stringLen - 1</t>
+  </si>
+  <si>
+    <t>public boolean findPalindrome(String s){</t>
+  </si>
+  <si>
+    <t>char[] arr = s.toCharArray();</t>
+  </si>
+  <si>
+    <t>int left = 0, right = s.length()-1;</t>
+  </si>
+  <si>
+    <t>while(left&lt;=right){</t>
+  </si>
+  <si>
+    <t>if(arr[left]!=arr[right]){</t>
+  </si>
+  <si>
+    <t>return false;</t>
+  </si>
+  <si>
+    <t>left++;</t>
+  </si>
+  <si>
+    <t>right--;</t>
+  </si>
+  <si>
+    <t>return true;</t>
+  </si>
+  <si>
+    <t>Find the 2nd Highest Number in a given Array</t>
+  </si>
+  <si>
+    <t>int[] arr = {8,3,5,4,9};</t>
+  </si>
+  <si>
+    <t>{5,4,3,2,1}</t>
+  </si>
+  <si>
+    <t>{1,2,3,4,5}</t>
+  </si>
+  <si>
+    <t>public int secondHighest(int[] arr){</t>
+  </si>
+  <si>
+    <t>int max = Integer.MIN_VALUE;</t>
+  </si>
+  <si>
+    <t>int secMax = 0;</t>
+  </si>
+  <si>
+    <t>for(int i = 0; i &lt; arr.length; i++){</t>
+  </si>
+  <si>
+    <t>if(arr[i]&gt;max){</t>
+  </si>
+  <si>
+    <t>secMax = max;</t>
+  </si>
+  <si>
+    <t>max = arr[i];</t>
+  </si>
+  <si>
+    <t>}else if(secMax &gt; arr[i]){</t>
+  </si>
+  <si>
+    <t>secMax = arr[i];</t>
+  </si>
+  <si>
+    <t>return secMax;</t>
+  </si>
+  <si>
+    <t>Find the Alternative Charaters which are same</t>
+  </si>
+  <si>
+    <t>String s "food" - return 0,"ffff" - return f,"abcd" - return null,</t>
+  </si>
+  <si>
+    <t>aabcdd - return a,d</t>
+  </si>
+  <si>
+    <t>public Set&lt;Character&gt; findNextRepeat(String s){</t>
+  </si>
+  <si>
+    <t>Set&lt;Character&gt; set = new HashSet&lt;Character&gt;();</t>
+  </si>
+  <si>
+    <t>for(int i = 0; i &lt; s.length()-1; i++){</t>
+  </si>
+  <si>
+    <t>if(s.charAt(i)==s.charAt(i+1)){</t>
+  </si>
+  <si>
+    <t>set.add(s.charAt(i));</t>
+  </si>
+  <si>
+    <t>return set;</t>
+  </si>
+  <si>
+    <t>Write XPath to get h2</t>
+  </si>
+  <si>
+    <t>"&lt; html&gt;&lt; h1&gt;&lt; body&gt;&lt; h2&gt;"</t>
+  </si>
+  <si>
+    <t>Given a Login Page. After entering UName and Pass, press Login</t>
+  </si>
+  <si>
+    <t>You will get a OTP. Wait untill you receive OTP.</t>
+  </si>
+  <si>
+    <t>public static void main(String args[]){</t>
+  </si>
+  <si>
+    <t>Webdriver driver = new ChromeDriver();</t>
+  </si>
+  <si>
+    <t>Webelement uname = driver.findElementByXpath("");</t>
+  </si>
+  <si>
+    <t>uname.sendKeys("username");</t>
+  </si>
+  <si>
+    <t>Webelement password = driver.findElementByXpath("");</t>
+  </si>
+  <si>
+    <t>password.sendKeys("******");</t>
+  </si>
+  <si>
+    <t>Webelement login = driver.findElementByXpath("");</t>
+  </si>
+  <si>
+    <t>login.click();</t>
+  </si>
+  <si>
+    <t>Wait wait = new FluentWait(driver).withTimeOut(30,SECONDS)</t>
+  </si>
+  <si>
+    <t>.pollingEvery(5,SECONDS)</t>
+  </si>
+  <si>
+    <t>.ignoring(NoSuchElementException.class);</t>
+  </si>
+  <si>
+    <t>Webelement otp = wait.until(ExpectedConditions.presenseOfElementLocated(By.XPath("otp"));</t>
+  </si>
+  <si>
+    <t>Table: Employee, Manager (Both Tables has Same Columns)</t>
+  </si>
+  <si>
+    <t>Columns: EmpId, Name, Role, Year, Salary</t>
+  </si>
+  <si>
+    <t>Find the Matching Occurence Between Employee Table and Manager Table</t>
+  </si>
+  <si>
+    <t>select *</t>
+  </si>
+  <si>
+    <t>from Employee A</t>
+  </si>
+  <si>
+    <t>inner join Manager B</t>
+  </si>
+  <si>
+    <t>on A.EmpId = B.EmpId</t>
+  </si>
+  <si>
+    <t>Find 2nd Max Salary:</t>
+  </si>
+  <si>
+    <t>select MAX(Salary) from Employee where Salary Not in (select MAX(Salary) from Employee)</t>
+  </si>
+  <si>
+    <t>Write a RestAssured Code to hit a POST request.</t>
+  </si>
+  <si>
+    <t>Find the Status Code and Parse the response.</t>
+  </si>
+  <si>
+    <t>RestAssured.baseURI = "requestURI";</t>
+  </si>
+  <si>
+    <t>RestAssured.authentication = RestAssured.basic("username","password");</t>
+  </si>
+  <si>
+    <t>Response response = RestAssured.given().post();</t>
+  </si>
+  <si>
+    <t>int statusCode = response.getStatusCode();</t>
+  </si>
+  <si>
+    <t>JsonPath json = response.jsonPath();</t>
+  </si>
+  <si>
+    <t>1. Reverse a String</t>
+  </si>
+  <si>
+    <t>2. Parse a JSON Response and find a whether address contains Banglore.</t>
+  </si>
+  <si>
+    <t>passengerName: "Rahul",</t>
+  </si>
+  <si>
+    <t>modeOfTravel: "Bus",</t>
+  </si>
+  <si>
+    <t>address: "Nagawara, Banglore"</t>
+  </si>
+  <si>
+    <t>RedBus Hiring Manager Questions:</t>
+  </si>
+  <si>
+    <t>Question 1:</t>
+  </si>
+  <si>
+    <t>Replace word 'in' with 'on'</t>
+  </si>
+  <si>
+    <t>Input:  Involved in Customer Interaction to identify Automatable Components</t>
+  </si>
+  <si>
+    <t>Output: Involved on Customer Interaction to identify Automatable Components</t>
+  </si>
+  <si>
+    <t>Ans:</t>
+  </si>
+  <si>
+    <t>public static void main(String[] args) throws IOException {</t>
+  </si>
+  <si>
+    <t>File file = new File("./Data/Input.txt");</t>
+  </si>
+  <si>
+    <t>BufferedReader br = new BufferedReader(new FileReader(file));</t>
+  </si>
+  <si>
+    <t>String line;</t>
+  </si>
+  <si>
+    <t>while((line=br.readLine())!=null) {</t>
+  </si>
+  <si>
+    <t>line = line.replaceAll("\\bin\\b", "on");</t>
+  </si>
+  <si>
+    <t>System.out.println(line);</t>
+  </si>
+  <si>
+    <t>br.close();</t>
+  </si>
+  <si>
+    <t>Question 2:</t>
+  </si>
+  <si>
+    <t>Assume we don't have Jenkins</t>
+  </si>
+  <si>
+    <t>We have a system where a build gets generated</t>
+  </si>
+  <si>
+    <t>We have another system where we have automation code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assume any Version Control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever there is a new build - automation should start on that build &amp; </t>
+  </si>
+  <si>
+    <t>should mail automation reports to X, Y, Z</t>
+  </si>
+  <si>
+    <t>How to do it?</t>
+  </si>
+  <si>
+    <t>Question 3:</t>
+  </si>
+  <si>
+    <t>Find the Largest Word in below String.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input: Designed and Developed Framework for UI Automation having Page Object Model </t>
+  </si>
+  <si>
+    <t>Implementation, Data Driven and TestNG</t>
+  </si>
+  <si>
+    <t>Ans: Implementation</t>
+  </si>
+  <si>
+    <t>Question 4:</t>
+  </si>
+  <si>
+    <t>Search your name in browser.</t>
+  </si>
+  <si>
+    <t>Press ctrl + F. You will get Number of occurences.</t>
+  </si>
+  <si>
+    <t>How will you do that in Selenium?</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>explain about product and business flows</t>
+  </si>
+  <si>
+    <t>few question from the resume</t>
+  </si>
+  <si>
+    <t>Test plan for we have a feature called ' deep discount which is like sort by low-high in Flipkart, and in any product, we have deep discount we will have a tag with the name f the bank for which discount is applicable for. come up with test plans for testing this feature</t>
+  </si>
+  <si>
+    <t>if the deep discount is not applying to the valid product how will you debug this</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>about yourself</t>
+  </si>
+  <si>
+    <t>Roles and responsibilities(in details)</t>
+  </si>
+  <si>
+    <t>had been into release management</t>
+  </si>
+  <si>
+    <t>explain about the product and 1 full sprint(to get how team works and our activities)</t>
+  </si>
+  <si>
+    <t>test plannig for our project</t>
+  </si>
+  <si>
+    <t>Types of mobile apps(native and hybrid)</t>
+  </si>
+  <si>
+    <t>what type of below mobile apps are</t>
+  </si>
+  <si>
+    <t>Whatsapp</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Debugging:</t>
+  </si>
+  <si>
+    <t>1)We have a delivery app(e.g. swiggy), we made an order in mobile app , but that is not showing up on the desktop version, how will we debug this</t>
+  </si>
+  <si>
+    <t>2)Login functionality is not working(upon clicking login button)</t>
+  </si>
+  <si>
+    <t>Given credentials are valid</t>
+  </si>
+  <si>
+    <t>network is good</t>
+  </si>
+  <si>
+    <t>Expected answer: Api</t>
+  </si>
+  <si>
+    <t>3) merchant have a calculator app which will calculate the amouunt to pay, and will have bluetooth connnectivity which will sycn with customer's mobile and customer can pay with using the app by clicking on 'Pay' or 'Decline' options(payment mode as only with wallet)</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Exactly this text: "father of OKRs"</t>
+  </si>
+  <si>
+    <t>OKR, Andrew Groove</t>
+  </si>
+  <si>
+    <t>Exactly this text: "father of OKRs"
+Not these words: OGSM</t>
+  </si>
+  <si>
+    <t>Andrew Groove</t>
+  </si>
+  <si>
+    <t>Exactly this text: "father of OKRs"
+One of these words: Hoshin</t>
+  </si>
+  <si>
+    <t>OKR</t>
+  </si>
+  <si>
+    <t>These words: starwars
+Exactly this text: "may the force be with you"
+Not these words: luke</t>
+  </si>
+  <si>
+    <t>Carrie Fisher</t>
+  </si>
+  <si>
+    <t>Exactly this text: "may the force be with you"
+Page title contains: rebel</t>
+  </si>
+  <si>
+    <t>List of Star Wars characters, List of Star Wars Rebels characters</t>
+  </si>
+  <si>
+    <t>2) Roles and Responsibility</t>
+  </si>
+  <si>
+    <t>3) Tools exposure</t>
+  </si>
+  <si>
+    <t>4) What enhancements you did to your framework</t>
+  </si>
+  <si>
+    <t>5) Enumerate case for https://developers.facebook.com/docs/pages/searching/ -&gt; this API</t>
+  </si>
+  <si>
+    <t>6) Given a set of characters, check whether a palindrom can be made or not. i/p -&gt; [m, m, a,a, d] -&gt; o/p -&gt; yes (since madam can be made)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/w/index.php?search=&amp;title=Special%3ASearch&amp;profile=advanced&amp;fulltext=1&amp;advancedSearch-current=%7B%7D&amp;ns0=1</t>
+  </si>
+  <si>
+    <t>2) Write POM script for below functionality</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>How will you handle a situation when you have goofed up big time, but the root cause/person behind the cause is unknown to the management?</t>
+  </si>
+  <si>
+    <t>What is more important – how others value you or how you value yourself?</t>
+  </si>
+  <si>
+    <t>Have you ever made a product or a test case finding sound better than it is, to market it?</t>
+  </si>
+  <si>
+    <t>What motivates you to come to the office each day? What are the activities that make you lose track of time?</t>
+  </si>
+  <si>
+    <t>What according to you was a breakthrough idea which you excelled/failed to sell to your manager? Why was it accepted/rejected and how did you feel about it?</t>
+  </si>
+  <si>
+    <t>You are about to deliver a project when you realize you have analyzed the wrong data and hence, produced faulty statistics. What would you do considering there is half the time left to do double work?</t>
+  </si>
+  <si>
+    <t>How do you set your goals? Describe your action plan to achieve them and your strategy when failing to do so.</t>
+  </si>
+  <si>
+    <t>Sum of given digit. 7852 -&gt; 22 -&gt; 4 (solve it in single loop)</t>
+  </si>
+  <si>
+    <t>Check whether the given string is palindrome or not. "madam" -&gt; true</t>
+  </si>
+  <si>
+    <t>Enumerate test case for below travel site,</t>
+  </si>
+  <si>
+    <t>Start location -&gt; To location -&gt; date picker -&gt; submit button -&gt; results</t>
+  </si>
+  <si>
+    <t>How will you test a dashboard which will have graphs or chart for travel site</t>
+  </si>
+  <si>
+    <t>Diff b/w / and // in xpath</t>
+  </si>
+  <si>
+    <t>What is REST API</t>
+  </si>
+  <si>
+    <t>Roles and Responsibilties</t>
+  </si>
+  <si>
+    <t>How you'll test in manual</t>
+  </si>
+  <si>
+    <t>How will you prioritize test cases to be automated</t>
+  </si>
+  <si>
+    <t>How will you say your framework is effective</t>
+  </si>
+  <si>
+    <t>What is the design used in your framework</t>
+  </si>
+  <si>
+    <t>1. Tools that you have used for API automation</t>
+  </si>
+  <si>
+    <t>2. Why to go for rest assured?</t>
+  </si>
+  <si>
+    <t>3. Explain about API framework</t>
+  </si>
+  <si>
+    <t>4. Reporting used for API framework</t>
+  </si>
+  <si>
+    <t>5. Write tests using restassured (reqres.in) for get and post</t>
+  </si>
+  <si>
+    <t>6. Write above tests using reusable functions (@beforemethod for reusable and @Test for actual test)</t>
+  </si>
+  <si>
+    <t>7. Use dataprovider and pass input to post request</t>
+  </si>
+  <si>
+    <t>8. Include assertions in above test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. run the tests using testng.xml from eclipse, from command line as testng xml and also from maven command line (include testng.xml in build goal and run from command line) </t>
+  </si>
+  <si>
+    <t>10. How do we debug different api error codes (eg. how to debug 500 error code)</t>
+  </si>
+  <si>
+    <t>11. How to deploy a java application in command line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. different AWS services </t>
+  </si>
+  <si>
+    <t>13. How to debug memory and Capacity issues</t>
+  </si>
+  <si>
+    <t>Where from?</t>
+  </si>
+  <si>
+    <t>Why left Cognizant or leaving current company?</t>
+  </si>
+  <si>
+    <t>Why ally?</t>
+  </si>
+  <si>
+    <t>What does ally do?</t>
+  </si>
+  <si>
+    <t>What is the biggest mistake you did in your life?</t>
+  </si>
+  <si>
+    <t>What is your future goal?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4028,16 +4588,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B7B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -4045,11 +4631,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4069,6 +4670,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4552,6 +5163,349 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B18DB3B-9D0D-4526-B1CF-6EF0A840E8A6}">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="71.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>755</v>
+      </c>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>756</v>
+      </c>
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>757</v>
+      </c>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>775</v>
+      </c>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>776</v>
+      </c>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>781</v>
+      </c>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>782</v>
+      </c>
+      <c r="B37" s="6"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B39" s="6"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>763</v>
+      </c>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>765</v>
+      </c>
+      <c r="B44" s="6"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>766</v>
+      </c>
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="B46" s="6"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="B48" s="6"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>769</v>
+      </c>
+      <c r="B49" s="6"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>770</v>
+      </c>
+      <c r="B50" s="6"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="B51" s="6"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6EED80-F386-4D8D-8E22-BBDE76B2048C}">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -4727,7 +5681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD1F9D0-1F41-4D46-A88C-38D4B372000A}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -4903,7 +5857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F27406-B35D-4E7F-BF58-232C7DFAD1A3}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -5038,7 +5992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CC4AA9-F201-4CF9-8C84-A706D3A63D28}">
   <dimension ref="A1:A55"/>
   <sheetViews>
@@ -5271,7 +6225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2778574C-63CC-463D-A68D-E4F793A5F3C8}">
   <dimension ref="A1:A56"/>
   <sheetViews>
@@ -5543,7 +6497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B7D59E-A1D8-4245-B8E3-CFBBD78B80F5}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -5646,7 +6600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9D4652-F80D-4003-93B0-0F8769751DA2}">
   <dimension ref="A1:A37"/>
   <sheetViews>
@@ -5847,7 +6801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B063943D-3BF7-4005-9BA4-776A95F07167}">
   <dimension ref="A2:A23"/>
   <sheetViews>
@@ -5968,7 +6922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31098C9C-93FE-485F-9190-A0148D218930}">
   <dimension ref="A1:A64"/>
   <sheetViews>
@@ -6286,77 +7240,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C33F1-A1FB-4B2B-8414-A0665D70F3A5}">
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="55.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>528</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70811466-9302-4B61-86B7-B701B3741742}">
   <dimension ref="A1:E239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+    <sheetView topLeftCell="B49" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -8137,6 +9025,72 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C33F1-A1FB-4B2B-8414-A0665D70F3A5}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="55.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>528</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073BA8A9-7826-4D89-BEBA-4976E18552D1}">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -8190,7 +9144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CEDD9D-03AE-426B-A47D-1BC31D89A7C9}">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -8280,7 +9234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277AEA5E-1693-4D23-AD99-E47AA3101B00}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -8470,7 +9424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75766EEF-6565-49DC-B14E-160310B644C5}">
   <dimension ref="A1:F60"/>
   <sheetViews>
@@ -9264,7 +10218,919 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5309C71-1A6A-4F8F-B38E-F8FF3A43BDC0}">
+  <dimension ref="A1:L110"/>
+  <sheetViews>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1315</v>
+      </c>
+      <c r="I4" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1316</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>1317</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>1318</v>
+      </c>
+      <c r="I8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>1323</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>1324</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>203</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1327</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K25" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K27" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>1331</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>1332</v>
+      </c>
+      <c r="K31" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>1333</v>
+      </c>
+      <c r="L32" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>1334</v>
+      </c>
+      <c r="L33" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>1335</v>
+      </c>
+      <c r="K34" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>1337</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>203</v>
+      </c>
+      <c r="J38" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>203</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>1339</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1340</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1342</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I50" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>203</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>1347</v>
+      </c>
+      <c r="I54" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>1348</v>
+      </c>
+      <c r="I57" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>1351</v>
+      </c>
+      <c r="I61" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>1352</v>
+      </c>
+      <c r="I63" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>1353</v>
+      </c>
+      <c r="I65" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D77" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D78" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7712651-353F-4F0A-8D24-BA2EA1B22FF3}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB6F42A-1102-41C7-8CFD-DB1D07A18272}">
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
+    <col min="2" max="2" width="45.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DD3467-2B99-44E2-94DD-B35AB2451446}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -9390,7 +11256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F02FB25-3DFF-41E7-92B5-834D40ACAD7B}">
   <dimension ref="A1:C96"/>
   <sheetViews>
@@ -10079,7 +11945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00A1B05-956D-4043-80BD-1DED8F2F6975}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -10329,7 +12195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB85AB0-402B-4E08-B2B3-647BD366FFAA}">
   <dimension ref="A1:B60"/>
   <sheetViews>
@@ -10686,7 +12552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA126997-88C6-42B8-AA54-B9F61EAF6019}">
   <dimension ref="A1:B45"/>
   <sheetViews>
@@ -10974,413 +12840,174 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE95AB5-C1FC-491D-8B54-702A2219AAD8}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B18DB3B-9D0D-4526-B1CF-6EF0A840E8A6}">
-  <dimension ref="A1:B55"/>
-  <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="71.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="61.6640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="47.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>173</v>
+      <c r="B1" s="2" t="s">
+        <v>1417</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>585</v>
+      <c r="A2" t="s">
+        <v>1073</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>694</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>586</v>
+      <c r="A3" t="s">
+        <v>1074</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>596</v>
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1075</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>597</v>
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1421</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>697</v>
+      <c r="A6" t="s">
+        <v>1077</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>698</v>
+      <c r="A7" t="s">
+        <v>1078</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>699</v>
+      <c r="A8" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>700</v>
+      <c r="A9" t="s">
+        <v>1080</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>703</v>
+      <c r="A10" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1082</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>704</v>
+      <c r="A13" s="2" t="s">
+        <v>1422</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>753</v>
-      </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>754</v>
-      </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>755</v>
-      </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>756</v>
-      </c>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>757</v>
-      </c>
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>758</v>
-      </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>759</v>
-      </c>
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>760</v>
-      </c>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>773</v>
-      </c>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>774</v>
-      </c>
-      <c r="B27" s="6"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>775</v>
-      </c>
-      <c r="B28" s="6"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>761</v>
-      </c>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>776</v>
-      </c>
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>778</v>
-      </c>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>779</v>
-      </c>
-      <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>781</v>
-      </c>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>782</v>
-      </c>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="B39" s="6"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>763</v>
-      </c>
-      <c r="B41" s="6"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>764</v>
-      </c>
-      <c r="B42" s="6"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>765</v>
-      </c>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>766</v>
-      </c>
-      <c r="B45" s="6"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>767</v>
-      </c>
-      <c r="B46" s="6"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>768</v>
-      </c>
-      <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>769</v>
-      </c>
-      <c r="B49" s="6"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
-        <v>770</v>
-      </c>
-      <c r="B50" s="6"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>771</v>
-      </c>
-      <c r="B51" s="6"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
-        <v>772</v>
-      </c>
-      <c r="B52" s="6"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="6"/>
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>1438</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>